<commit_message>
notes after data meeting with kate
</commit_message>
<xml_diff>
--- a/Data-Info.xlsx
+++ b/Data-Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuart/ea_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB91098-198D-F743-839F-AEFACFDC39A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647042C2-561F-AC41-9C82-9DF846585DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12580" yWindow="4160" windowWidth="21240" windowHeight="16400" xr2:uid="{78CF829B-A9BE-8D4D-A6FC-B99E30F29951}"/>
+    <workbookView xWindow="4400" yWindow="980" windowWidth="21240" windowHeight="16400" xr2:uid="{78CF829B-A9BE-8D4D-A6FC-B99E30F29951}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Daily</t>
   </si>
   <si>
-    <t>1/1/2000 to 1/9/2010</t>
-  </si>
-  <si>
     <t>2859TH daily flow</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>No Data</t>
+  </si>
+  <si>
+    <t>1/1/2000 to present</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -544,7 +544,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -561,7 +561,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -586,84 +586,84 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ignoring images and adding more to metadata table
</commit_message>
<xml_diff>
--- a/Data-Info.xlsx
+++ b/Data-Info.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuart/ea_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647042C2-561F-AC41-9C82-9DF846585DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393474B4-DE35-4046-AC28-5DF5103A38E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="980" windowWidth="21240" windowHeight="16400" xr2:uid="{78CF829B-A9BE-8D4D-A6FC-B99E30F29951}"/>
+    <workbookView xWindow="4400" yWindow="980" windowWidth="21240" windowHeight="16400" activeTab="1" xr2:uid="{78CF829B-A9BE-8D4D-A6FC-B99E30F29951}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quantity" sheetId="1" r:id="rId1"/>
+    <sheet name="Quality" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="95">
   <si>
     <t>Location</t>
   </si>
@@ -121,6 +122,195 @@
   </si>
   <si>
     <t>1/1/2000 to present</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_0076.csv</t>
+  </si>
+  <si>
+    <t>2000-01-11T10:45:00</t>
+  </si>
+  <si>
+    <t>2012-11-28T14:45:00</t>
+  </si>
+  <si>
+    <t>Temp Water</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_0077.csv</t>
+  </si>
+  <si>
+    <t>2010-06-03T10:30:00</t>
+  </si>
+  <si>
+    <t>Cond @ 25C</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_0085.csv</t>
+  </si>
+  <si>
+    <t>2007-12-03T12:17:00</t>
+  </si>
+  <si>
+    <t>BOD ATU</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_0117.csv</t>
+  </si>
+  <si>
+    <t>2003-01-17T10:50:00</t>
+  </si>
+  <si>
+    <t>Nitrate-N</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_9901.csv</t>
+  </si>
+  <si>
+    <t>O Diss %sat</t>
+  </si>
+  <si>
+    <t>TH-PCNR0014_9924.csv</t>
+  </si>
+  <si>
+    <t>Oxygen Diss</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0015_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0207_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0012_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0013_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0020_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0019_9924.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_0076.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_0077.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_0085.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_0117.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_9901.csv</t>
+  </si>
+  <si>
+    <t>TH-PCNR0145_9924.csv</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>Determinand</t>
   </si>
 </sst>
 </file>
@@ -483,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95840FB8-B14E-E14A-9F60-AE5CCE3E59B9}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,4 +859,710 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E131A5-474E-DA4F-ADE9-4585E011C35D}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>